<commit_message>
Changes in SelectElementWrapper, added comment in WebElementWrapper, added DriverCommandsTests.cs file and added tests to DriverWrapperTests.cs and DemoTests.cs files.
</commit_message>
<xml_diff>
--- a/SeleniumCSharp/Resources/TestCaseData.xlsx
+++ b/SeleniumCSharp/Resources/TestCaseData.xlsx
@@ -43,7 +43,7 @@
     <t>Teacher</t>
   </si>
   <si>
-    <t>vjteacher</t>
+    <t>vj_teacher</t>
   </si>
 </sst>
 </file>
@@ -385,7 +385,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>